<commit_message>
[feature] UI background | Files: Produktionssteuerungssystem.xlsx, Project/SmoothMainWindow.xaml, Project/SmoothMainWindow.xaml.cs
</commit_message>
<xml_diff>
--- a/Produktionssteuerungssystem.xlsx
+++ b/Produktionssteuerungssystem.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr dateCompatibility="0" filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:19_{57CEE83F-DD74-42E2-90E1-21BEC81BFEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{A8E6E1E6-BC51-4648-869D-6A96071D1310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="12960" windowHeight="15360" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -1367,13 +1367,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15361" name="Scroll Bar 1" descr="Scrollbar for scrolling through the Gantt Timeline.">
+        <xdr:cNvPr id="16385" name="Scroll Bar 1" descr="Scrollbar for scrolling through the Gantt Timeline.">
           <a:extLst>
             <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
               <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s15361"/>
             </a:ext>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000013C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C3E52F6-C3EE-D922-B79A-7F6F58D59B5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1388,11 +1388,24 @@
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln w="9525">
-          <a:miter lim="800%"/>
-          <a:headEnd/>
-          <a:tailEnd/>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:noFill/>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:noFill/>
+              <a:miter lim="800%"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
@@ -1764,8 +1777,8 @@
   </sheetPr>
   <dimension ref="A1:BK36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A12" zoomScale="98" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A14" zoomScale="98" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="30" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.5"/>
@@ -1934,7 +1947,7 @@
       </c>
       <c r="C5" s="38" t="d">
         <f ca="1">IFERROR(IF(MIN(Milestones34[Start])=0,TODAY(),MIN(Milestones34[Start])),TODAY())</f>
-        <v>2025-01-27</v>
+        <v>2025-03-03</v>
       </c>
       <c r="E5" s="44"/>
       <c r="H5" s="29"/>
@@ -1970,7 +1983,7 @@
       </c>
       <c r="H6" s="52" t="str">
         <f ca="1">TEXT(H7,"mmmm")</f>
-        <v>January</v>
+        <v>March</v>
       </c>
       <c r="I6" s="52"/>
       <c r="J6" s="52"/>
@@ -1980,7 +1993,7 @@
       <c r="N6" s="25"/>
       <c r="O6" s="25" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v>February</v>
+        <v/>
       </c>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
@@ -2010,7 +2023,7 @@
       <c r="AI6" s="25"/>
       <c r="AJ6" s="53" t="str">
         <f ca="1">IF(OR(TEXT(AJ7,"mmmm")=AC6,TEXT(AJ7,"mmmm")=V6,TEXT(AJ7,"mmmm")=O6,TEXT(AJ7,"mmmm")=H6),"",TEXT(AJ7,"mmmm"))</f>
-        <v/>
+        <v>April</v>
       </c>
       <c r="AK6" s="53"/>
       <c r="AL6" s="53"/>
@@ -2020,7 +2033,7 @@
       <c r="AP6" s="25"/>
       <c r="AQ6" s="25" t="str">
         <f ca="1">IF(OR(TEXT(AQ7,"mmmm")=AJ6,TEXT(AQ7,"mmmm")=AC6,TEXT(AQ7,"mmmm")=V6,TEXT(AQ7,"mmmm")=O6),"",TEXT(AQ7,"mmmm"))</f>
-        <v>March</v>
+        <v/>
       </c>
       <c r="AR6" s="25"/>
       <c r="AS6" s="25"/>
@@ -2054,227 +2067,227 @@
       <c r="B7" s="23"/>
       <c r="H7" s="68" t="d">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>2025-01-29</v>
+        <v>2025-03-05</v>
       </c>
       <c r="I7" s="69" t="d">
         <f ca="1">H7+1</f>
-        <v>2025-01-30</v>
+        <v>2025-03-06</v>
       </c>
       <c r="J7" s="69" t="d">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>2025-01-31</v>
+        <v>2025-03-07</v>
       </c>
       <c r="K7" s="69" t="d">
         <f ca="1">J7+1</f>
-        <v>2025-02-01</v>
+        <v>2025-03-08</v>
       </c>
       <c r="L7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-02</v>
+        <v>2025-03-09</v>
       </c>
       <c r="M7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-03</v>
+        <v>2025-03-10</v>
       </c>
       <c r="N7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-04</v>
+        <v>2025-03-11</v>
       </c>
       <c r="O7" s="69" t="d">
         <f ca="1">N7+1</f>
-        <v>2025-02-05</v>
+        <v>2025-03-12</v>
       </c>
       <c r="P7" s="69" t="d">
         <f ca="1">O7+1</f>
-        <v>2025-02-06</v>
+        <v>2025-03-13</v>
       </c>
       <c r="Q7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-07</v>
+        <v>2025-03-14</v>
       </c>
       <c r="R7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-08</v>
+        <v>2025-03-15</v>
       </c>
       <c r="S7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-09</v>
+        <v>2025-03-16</v>
       </c>
       <c r="T7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-10</v>
+        <v>2025-03-17</v>
       </c>
       <c r="U7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-11</v>
+        <v>2025-03-18</v>
       </c>
       <c r="V7" s="69" t="d">
         <f ca="1">U7+1</f>
-        <v>2025-02-12</v>
+        <v>2025-03-19</v>
       </c>
       <c r="W7" s="69" t="d">
         <f ca="1">V7+1</f>
-        <v>2025-02-13</v>
+        <v>2025-03-20</v>
       </c>
       <c r="X7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-14</v>
+        <v>2025-03-21</v>
       </c>
       <c r="Y7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-15</v>
+        <v>2025-03-22</v>
       </c>
       <c r="Z7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-16</v>
+        <v>2025-03-23</v>
       </c>
       <c r="AA7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-17</v>
+        <v>2025-03-24</v>
       </c>
       <c r="AB7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-18</v>
+        <v>2025-03-25</v>
       </c>
       <c r="AC7" s="69" t="d">
         <f ca="1">AB7+1</f>
-        <v>2025-02-19</v>
+        <v>2025-03-26</v>
       </c>
       <c r="AD7" s="69" t="d">
         <f ca="1">AC7+1</f>
-        <v>2025-02-20</v>
+        <v>2025-03-27</v>
       </c>
       <c r="AE7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-21</v>
+        <v>2025-03-28</v>
       </c>
       <c r="AF7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-22</v>
+        <v>2025-03-29</v>
       </c>
       <c r="AG7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-23</v>
+        <v>2025-03-30</v>
       </c>
       <c r="AH7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-24</v>
+        <v>2025-03-31</v>
       </c>
       <c r="AI7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-25</v>
+        <v>2025-04-01</v>
       </c>
       <c r="AJ7" s="69" t="d">
         <f ca="1">AI7+1</f>
-        <v>2025-02-26</v>
+        <v>2025-04-02</v>
       </c>
       <c r="AK7" s="69" t="d">
         <f ca="1">AJ7+1</f>
-        <v>2025-02-27</v>
+        <v>2025-04-03</v>
       </c>
       <c r="AL7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-02-28</v>
+        <v>2025-04-04</v>
       </c>
       <c r="AM7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-01</v>
+        <v>2025-04-05</v>
       </c>
       <c r="AN7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-02</v>
+        <v>2025-04-06</v>
       </c>
       <c r="AO7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-03</v>
+        <v>2025-04-07</v>
       </c>
       <c r="AP7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-04</v>
+        <v>2025-04-08</v>
       </c>
       <c r="AQ7" s="69" t="d">
         <f ca="1">AP7+1</f>
-        <v>2025-03-05</v>
+        <v>2025-04-09</v>
       </c>
       <c r="AR7" s="69" t="d">
         <f ca="1">AQ7+1</f>
-        <v>2025-03-06</v>
+        <v>2025-04-10</v>
       </c>
       <c r="AS7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-07</v>
+        <v>2025-04-11</v>
       </c>
       <c r="AT7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-08</v>
+        <v>2025-04-12</v>
       </c>
       <c r="AU7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-09</v>
+        <v>2025-04-13</v>
       </c>
       <c r="AV7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-10</v>
+        <v>2025-04-14</v>
       </c>
       <c r="AW7" s="69" t="d">
         <f t="shared" ca="1" si="0"/>
-        <v>2025-03-11</v>
+        <v>2025-04-15</v>
       </c>
       <c r="AX7" s="69" t="d">
         <f ca="1">AW7+1</f>
-        <v>2025-03-12</v>
+        <v>2025-04-16</v>
       </c>
       <c r="AY7" s="69" t="d">
         <f ca="1">AX7+1</f>
-        <v>2025-03-13</v>
+        <v>2025-04-17</v>
       </c>
       <c r="AZ7" s="69" t="d">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>2025-03-14</v>
+        <v>2025-04-18</v>
       </c>
       <c r="BA7" s="69" t="d">
         <f t="shared" ca="1" si="1"/>
-        <v>2025-03-15</v>
+        <v>2025-04-19</v>
       </c>
       <c r="BB7" s="69" t="d">
         <f t="shared" ca="1" si="1"/>
-        <v>2025-03-16</v>
+        <v>2025-04-20</v>
       </c>
       <c r="BC7" s="69" t="d">
         <f t="shared" ca="1" si="1"/>
-        <v>2025-03-17</v>
+        <v>2025-04-21</v>
       </c>
       <c r="BD7" s="69" t="d">
         <f t="shared" ca="1" si="1"/>
-        <v>2025-03-18</v>
+        <v>2025-04-22</v>
       </c>
       <c r="BE7" s="69" t="d">
         <f ca="1">BD7+1</f>
-        <v>2025-03-19</v>
+        <v>2025-04-23</v>
       </c>
       <c r="BF7" s="69" t="d">
         <f ca="1">BE7+1</f>
-        <v>2025-03-20</v>
+        <v>2025-04-24</v>
       </c>
       <c r="BG7" s="69" t="d">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>2025-03-21</v>
+        <v>2025-04-25</v>
       </c>
       <c r="BH7" s="69" t="d">
         <f t="shared" ca="1" si="2"/>
-        <v>2025-03-22</v>
+        <v>2025-04-26</v>
       </c>
       <c r="BI7" s="69" t="d">
         <f t="shared" ca="1" si="2"/>
-        <v>2025-03-23</v>
+        <v>2025-04-27</v>
       </c>
       <c r="BJ7" s="69" t="d">
         <f t="shared" ca="1" si="2"/>
-        <v>2025-03-24</v>
+        <v>2025-04-28</v>
       </c>
       <c r="BK7" s="70" t="d">
         <f t="shared" ca="1" si="2"/>
-        <v>2025-03-25</v>
+        <v>2025-04-29</v>
       </c>
     </row>
     <row r="8" spans="1:63" ht="31.1" customHeight="1" x14ac:dyDescent="0.5">
@@ -2825,11 +2838,11 @@
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="64">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E11" s="35" t="d">
         <f ca="1">TODAY() -7</f>
-        <v>2025-01-27</v>
+        <v>2025-03-03</v>
       </c>
       <c r="F11" s="16">
         <v>9</v>
@@ -3066,10 +3079,12 @@
         <v>24</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="64"/>
+      <c r="D12" s="64">
+        <v>1</v>
+      </c>
       <c r="E12" s="35" t="d">
         <f ca="1">TODAY()+5</f>
-        <v>2025-02-08</v>
+        <v>2025-03-15</v>
       </c>
       <c r="F12" s="16">
         <v>5</v>
@@ -3311,7 +3326,7 @@
       </c>
       <c r="E13" s="35" t="d">
         <f ca="1">TODAY()-3</f>
-        <v>2025-01-31</v>
+        <v>2025-03-07</v>
       </c>
       <c r="F13" s="16">
         <v>15</v>
@@ -3548,10 +3563,12 @@
         <v>26</v>
       </c>
       <c r="C14" s="17"/>
-      <c r="D14" s="64"/>
+      <c r="D14" s="64">
+        <v>0.8</v>
+      </c>
       <c r="E14" s="35" t="d">
         <f ca="1">TODAY()+20</f>
-        <v>2025-02-23</v>
+        <v>2025-03-30</v>
       </c>
       <c r="F14" s="16">
         <v>1</v>
@@ -3793,7 +3810,7 @@
       </c>
       <c r="E15" s="35" t="d">
         <f ca="1">TODAY()+6</f>
-        <v>2025-02-09</v>
+        <v>2025-03-16</v>
       </c>
       <c r="F15" s="16">
         <v>6</v>
@@ -4268,7 +4285,7 @@
       <c r="D17" s="64"/>
       <c r="E17" s="35" t="d">
         <f ca="1">TODAY()+15</f>
-        <v>2025-02-18</v>
+        <v>2025-03-25</v>
       </c>
       <c r="F17" s="16">
         <v>4</v>
@@ -4508,7 +4525,7 @@
       <c r="D18" s="64"/>
       <c r="E18" s="35" t="d">
         <f ca="1">TODAY()+19</f>
-        <v>2025-02-22</v>
+        <v>2025-03-29</v>
       </c>
       <c r="F18" s="16">
         <v>14</v>
@@ -4748,7 +4765,7 @@
       <c r="D19" s="64"/>
       <c r="E19" s="35" t="d">
         <f ca="1">TODAY()+35</f>
-        <v>2025-03-10</v>
+        <v>2025-04-14</v>
       </c>
       <c r="F19" s="16">
         <v>6</v>
@@ -4988,7 +5005,7 @@
       <c r="D20" s="64"/>
       <c r="E20" s="35" t="d">
         <f ca="1">TODAY()+48</f>
-        <v>2025-03-23</v>
+        <v>2025-04-27</v>
       </c>
       <c r="F20" s="16">
         <v>3</v>
@@ -5225,10 +5242,12 @@
         <v>22</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="64"/>
+      <c r="D21" s="64">
+        <v>0.1</v>
+      </c>
       <c r="E21" s="35" t="d">
         <f ca="1">TODAY()</f>
-        <v>2025-02-03</v>
+        <v>2025-03-10</v>
       </c>
       <c r="F21" s="16">
         <v>120</v>
@@ -5703,7 +5722,7 @@
       <c r="D23" s="64"/>
       <c r="E23" s="35" t="d">
         <f ca="1">TODAY()+37</f>
-        <v>2025-03-12</v>
+        <v>2025-04-16</v>
       </c>
       <c r="F23" s="16">
         <v>15</v>
@@ -5943,7 +5962,7 @@
       <c r="D24" s="64"/>
       <c r="E24" s="35" t="d">
         <f ca="1">TODAY()+29</f>
-        <v>2025-03-04</v>
+        <v>2025-04-08</v>
       </c>
       <c r="F24" s="16">
         <v>5</v>
@@ -6183,7 +6202,7 @@
       <c r="D25" s="64"/>
       <c r="E25" s="35" t="d">
         <f ca="1">TODAY()+80</f>
-        <v>2025-04-24</v>
+        <v>2025-05-29</v>
       </c>
       <c r="F25" s="16">
         <v>5</v>
@@ -8678,7 +8697,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <controls>
-    <control shapeId="15361" r:id="rId4" name="Scroll Bar 1">
+    <control shapeId="16385" r:id="rId4" name="Scroll Bar 1">
       <controlPr defaultSize="0" autoPict="0" altText="Scrollbar for scrolling through the Gantt Timeline.">
         <anchor moveWithCells="1">
           <from>
@@ -8896,35 +8915,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9224,27 +9214,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{115E488A-90BD-4FEC-9F20-FFAF098D38E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{FF8EE784-10F3-46EF-B6DC-D206373B3A17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{D999942B-3CC5-4007-B7B6-6870B5EC1C9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9265,6 +9264,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{FF8EE784-10F3-46EF-B6DC-D206373B3A17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{115E488A-90BD-4FEC-9F20-FFAF098D38E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>